<commit_message>
1. Added threaded observeables 2. removed redundant files
</commit_message>
<xml_diff>
--- a/dist/artifacts/msg_enum.xlsx
+++ b/dist/artifacts/msg_enum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWAK_APD_CARE\apdcare\therapy_src\scripts\code_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDE17AF-DF1E-42F2-8DA2-0E75A223A9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D512EE40-D62A-420C-9E8B-31DF594821F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="12" xr2:uid="{9845A9FD-3F8D-4BE4-B40E-983F7B836130}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{9845A9FD-3F8D-4BE4-B40E-983F7B836130}"/>
   </bookViews>
   <sheets>
     <sheet name="threads" sheetId="2" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="528">
   <si>
     <t>thread_cmd</t>
   </si>
@@ -1653,6 +1653,9 @@
   </si>
   <si>
     <t>MSG_UC_MASTER_EXEC_UC_RUN_THERAPY</t>
+  </si>
+  <si>
+    <t>UNSET_CFG</t>
   </si>
 </sst>
 </file>
@@ -2351,7 +2354,7 @@
   <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2610,7 +2613,7 @@
         <v>118</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -3530,7 +3533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75AE531-5F28-4AEB-8C78-A2C7D800AE06}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -4498,10 +4501,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAF780E-2E2E-429F-8006-84B4BA367FA4}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4549,7 +4552,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -4557,24 +4560,29 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
+        <v>527</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>369</v>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4728,7 +4736,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4931,7 +4939,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5144,7 +5152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C02AF99-CC81-4E23-AD37-6DA0EA50F8B4}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1. added sensors override tab
</commit_message>
<xml_diff>
--- a/dist/artifacts/msg_enum.xlsx
+++ b/dist/artifacts/msg_enum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWAK_APD_CARE\apdcare\therapy_src\scripts\code_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D512EE40-D62A-420C-9E8B-31DF594821F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC8D4DB-6496-42DE-8B7A-920DC22DCBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{9845A9FD-3F8D-4BE4-B40E-983F7B836130}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="12" xr2:uid="{9845A9FD-3F8D-4BE4-B40E-983F7B836130}"/>
   </bookViews>
   <sheets>
     <sheet name="threads" sheetId="2" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="536">
   <si>
     <t>thread_cmd</t>
   </si>
@@ -1656,6 +1656,30 @@
   </si>
   <si>
     <t>UNSET_CFG</t>
+  </si>
+  <si>
+    <t>MSG_SENSORS_SET_BUBBLE_DET_VAL</t>
+  </si>
+  <si>
+    <t>MSG_SENSORS_UNSET_BUBBLE_DET_VAL</t>
+  </si>
+  <si>
+    <t>trig_set_level_val</t>
+  </si>
+  <si>
+    <t>trig_unset_level_val</t>
+  </si>
+  <si>
+    <t>Level value overridden</t>
+  </si>
+  <si>
+    <t>Level set value failed</t>
+  </si>
+  <si>
+    <t>Level value real time</t>
+  </si>
+  <si>
+    <t>Level real time failed</t>
   </si>
 </sst>
 </file>
@@ -2353,8 +2377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67343738-2015-487A-BA26-ADA61FE35773}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2614,6 +2638,9 @@
       </c>
       <c r="E13">
         <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -3531,10 +3558,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75AE531-5F28-4AEB-8C78-A2C7D800AE06}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3928,7 +3955,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>147</v>
+        <v>528</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3936,16 +3963,19 @@
       <c r="C20">
         <v>1</v>
       </c>
+      <c r="D20" t="s">
+        <v>530</v>
+      </c>
       <c r="E20" t="s">
-        <v>148</v>
+        <v>532</v>
       </c>
       <c r="F20" t="s">
-        <v>149</v>
+        <v>533</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>456</v>
+        <v>529</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3954,18 +3984,18 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>457</v>
+        <v>531</v>
       </c>
       <c r="E21" t="s">
-        <v>458</v>
+        <v>534</v>
       </c>
       <c r="F21" t="s">
-        <v>459</v>
+        <v>535</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3973,19 +4003,16 @@
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
-        <v>177</v>
-      </c>
       <c r="E22" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="F22" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>300</v>
+        <v>456</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3994,18 +4021,18 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>302</v>
+        <v>457</v>
       </c>
       <c r="E23" t="s">
-        <v>306</v>
+        <v>458</v>
       </c>
       <c r="F23" t="s">
-        <v>310</v>
+        <v>459</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>301</v>
+        <v>178</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4014,18 +4041,18 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>302</v>
+        <v>177</v>
       </c>
       <c r="E24" t="s">
-        <v>307</v>
+        <v>180</v>
       </c>
       <c r="F24" t="s">
-        <v>311</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -4034,18 +4061,18 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="E25" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="F25" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>449</v>
+        <v>301</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4054,18 +4081,18 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>450</v>
+        <v>302</v>
       </c>
       <c r="E26" t="s">
-        <v>451</v>
+        <v>307</v>
       </c>
       <c r="F26" t="s">
-        <v>452</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -4074,18 +4101,18 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="E27" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="F27" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>304</v>
+        <v>449</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4094,18 +4121,18 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>352</v>
+        <v>450</v>
       </c>
       <c r="E28" t="s">
-        <v>309</v>
+        <v>451</v>
       </c>
       <c r="F28" t="s">
-        <v>313</v>
+        <v>452</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>329</v>
+        <v>303</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -4114,18 +4141,18 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>339</v>
+        <v>305</v>
       </c>
       <c r="E29" t="s">
-        <v>338</v>
+        <v>308</v>
       </c>
       <c r="F29" t="s">
-        <v>337</v>
+        <v>312</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -4134,18 +4161,18 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>340</v>
+        <v>352</v>
       </c>
       <c r="E30" t="s">
-        <v>514</v>
+        <v>309</v>
       </c>
       <c r="F30" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -4154,18 +4181,18 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="E31" t="s">
-        <v>512</v>
+        <v>338</v>
       </c>
       <c r="F31" t="s">
-        <v>513</v>
+        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>524</v>
+        <v>330</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -4174,18 +4201,18 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>509</v>
+        <v>340</v>
       </c>
       <c r="E32" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F32" t="s">
-        <v>516</v>
+        <v>343</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>525</v>
+        <v>331</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -4194,18 +4221,18 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>510</v>
+        <v>348</v>
       </c>
       <c r="E33" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="F33" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -4214,18 +4241,18 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E34" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="F34" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>332</v>
+        <v>525</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -4234,18 +4261,18 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>341</v>
+        <v>510</v>
       </c>
       <c r="E35" t="s">
-        <v>344</v>
+        <v>517</v>
       </c>
       <c r="F35" t="s">
-        <v>345</v>
+        <v>518</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>333</v>
+        <v>526</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -4254,12 +4281,18 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>349</v>
+        <v>511</v>
+      </c>
+      <c r="E36" t="s">
+        <v>519</v>
+      </c>
+      <c r="F36" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -4268,18 +4301,18 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E37" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F37" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -4288,12 +4321,12 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -4302,12 +4335,18 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>351</v>
+        <v>342</v>
+      </c>
+      <c r="E39" t="s">
+        <v>346</v>
+      </c>
+      <c r="F39" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>353</v>
+        <v>335</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -4316,18 +4355,12 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>356</v>
-      </c>
-      <c r="E40" t="s">
-        <v>359</v>
-      </c>
-      <c r="F40" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>354</v>
+        <v>336</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -4336,18 +4369,12 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>357</v>
-      </c>
-      <c r="E41" t="s">
-        <v>361</v>
-      </c>
-      <c r="F41" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -4356,18 +4383,18 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E42" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F42" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>453</v>
+        <v>354</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -4376,18 +4403,18 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E43" t="s">
-        <v>454</v>
+        <v>361</v>
       </c>
       <c r="F43" t="s">
-        <v>455</v>
+        <v>360</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -4396,18 +4423,18 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E44" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="F44" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -4416,18 +4443,18 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>462</v>
+        <v>358</v>
       </c>
       <c r="E45" t="s">
-        <v>372</v>
+        <v>454</v>
       </c>
       <c r="F45" t="s">
-        <v>373</v>
+        <v>455</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>461</v>
+        <v>370</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -4436,7 +4463,7 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>463</v>
+        <v>371</v>
       </c>
       <c r="E46" t="s">
         <v>372</v>
@@ -4447,21 +4474,61 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>460</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>462</v>
+      </c>
+      <c r="E47" t="s">
+        <v>372</v>
+      </c>
+      <c r="F47" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>461</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>463</v>
+      </c>
+      <c r="E48" t="s">
+        <v>372</v>
+      </c>
+      <c r="F48" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>464</v>
       </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
         <v>465</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E49" t="s">
         <v>466</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F49" t="s">
         <v>467</v>
       </c>
     </row>
@@ -4503,7 +4570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAF780E-2E2E-429F-8006-84B4BA367FA4}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1. Added rx as content
</commit_message>
<xml_diff>
--- a/dist/artifacts/msg_enum.xlsx
+++ b/dist/artifacts/msg_enum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWAK_APD_CARE\apdcare\therapy_src\scripts\code_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC8D4DB-6496-42DE-8B7A-920DC22DCBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7CF3D0-5384-4B5B-BDA4-E99D95651CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="12" xr2:uid="{9845A9FD-3F8D-4BE4-B40E-983F7B836130}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="11" xr2:uid="{9845A9FD-3F8D-4BE4-B40E-983F7B836130}"/>
   </bookViews>
   <sheets>
     <sheet name="threads" sheetId="2" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="533">
   <si>
     <t>thread_cmd</t>
   </si>
@@ -437,30 +437,6 @@
     <t>valve move time</t>
   </si>
   <si>
-    <t>MSG_SENSORS_GET_FP1_LPF_WIN_SIZE</t>
-  </si>
-  <si>
-    <t>fp1 lpf size</t>
-  </si>
-  <si>
-    <t>MSG_SENSORS_GET_FP1_RUN_INTERVAL</t>
-  </si>
-  <si>
-    <t>fp1 sample time</t>
-  </si>
-  <si>
-    <t>MSG_SENSORS_GET_FP2_LPF_WIN_SIZE</t>
-  </si>
-  <si>
-    <t>fp2 lpf size</t>
-  </si>
-  <si>
-    <t>MSG_SENSORS_GET_FP2_RUN_INTERVAL</t>
-  </si>
-  <si>
-    <t>fp2 sample time</t>
-  </si>
-  <si>
     <t>MSG_SENSORS_GET_TURB_TOP_RUN_INTERVAL</t>
   </si>
   <si>
@@ -1680,6 +1656,21 @@
   </si>
   <si>
     <t>Level real time failed</t>
+  </si>
+  <si>
+    <t>TX_LOG_CFG_1T</t>
+  </si>
+  <si>
+    <t>TX_LOG_CFG_ALL</t>
+  </si>
+  <si>
+    <t>HT_MODE</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>off</t>
   </si>
 </sst>
 </file>
@@ -2108,7 +2099,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -2129,10 +2120,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9376E3EC-A3EF-4E74-A008-13FD454F2D6B}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D1" sqref="D1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2142,7 +2133,7 @@
     <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -2152,8 +2143,12 @@
       <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2161,33 +2156,43 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2199,10 +2204,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB8DE98-D929-4CE5-A1B4-9DDCBFC59D47}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2210,10 +2215,10 @@
     <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -2224,147 +2229,148 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>356</v>
+      </c>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C3" t="s">
         <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" t="s">
+        <v>513</v>
+      </c>
+      <c r="D6" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" t="s">
+        <v>514</v>
+      </c>
+      <c r="D7" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C8" t="s">
+        <v>515</v>
+      </c>
+      <c r="D8" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>204</v>
       </c>
-      <c r="C4" t="s">
-        <v>225</v>
-      </c>
-      <c r="D4" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="C12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>205</v>
       </c>
-      <c r="C5" t="s">
-        <v>228</v>
-      </c>
-      <c r="D5" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="C13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>206</v>
       </c>
-      <c r="C6" t="s">
-        <v>521</v>
-      </c>
-      <c r="D6" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>207</v>
       </c>
-      <c r="C7" t="s">
-        <v>522</v>
-      </c>
-      <c r="D7" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>208</v>
-      </c>
-      <c r="C8" t="s">
-        <v>523</v>
-      </c>
-      <c r="D8" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>209</v>
-      </c>
-      <c r="C9" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>210</v>
-      </c>
-      <c r="C10" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>211</v>
-      </c>
-      <c r="C11" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>212</v>
-      </c>
-      <c r="C12" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>213</v>
-      </c>
-      <c r="C13" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2375,10 +2381,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67343738-2015-487A-BA26-ADA61FE35773}">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2389,7 +2395,7 @@
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
@@ -2406,7 +2412,7 @@
         <v>87</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="G1" s="1">
         <v>0</v>
@@ -2414,8 +2420,11 @@
       <c r="H1" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1">
+        <v>65535</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -2432,7 +2441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -2449,10 +2458,10 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -2469,7 +2478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>96</v>
       </c>
@@ -2486,7 +2495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -2503,10 +2512,10 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>102</v>
       </c>
@@ -2523,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -2540,10 +2549,10 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -2560,10 +2569,10 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -2580,10 +2589,10 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>112</v>
       </c>
@@ -2600,10 +2609,10 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -2620,10 +2629,10 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -2640,10 +2649,10 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -2660,24 +2669,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>121</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
         <v>122</v>
       </c>
       <c r="D15" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -2730,818 +2739,762 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="B19" t="s">
         <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="B20" t="s">
         <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="B21" t="s">
         <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="D21" t="s">
         <v>105</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>186</v>
+      </c>
+      <c r="G21" t="s">
+        <v>209</v>
+      </c>
+      <c r="H21" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D23" t="s">
-        <v>165</v>
+        <v>105</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D24" t="s">
-        <v>165</v>
+        <v>105</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>161</v>
+        <v>495</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>497</v>
       </c>
       <c r="C25" t="s">
-        <v>164</v>
+        <v>498</v>
       </c>
       <c r="D25" t="s">
-        <v>105</v>
+        <v>412</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>194</v>
-      </c>
-      <c r="G25" t="s">
-        <v>217</v>
-      </c>
-      <c r="H25" t="s">
-        <v>218</v>
+        <v>494</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>153</v>
+        <v>496</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>497</v>
       </c>
       <c r="C26" t="s">
-        <v>156</v>
+        <v>499</v>
       </c>
       <c r="D26" t="s">
-        <v>105</v>
+        <v>412</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>196</v>
+        <v>500</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>154</v>
+        <v>275</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>175</v>
       </c>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>246</v>
       </c>
       <c r="D27" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>197</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>155</v>
+        <v>276</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>175</v>
       </c>
       <c r="C28" t="s">
-        <v>158</v>
+        <v>247</v>
       </c>
       <c r="D28" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>195</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>503</v>
+        <v>280</v>
       </c>
       <c r="B29" t="s">
-        <v>505</v>
+        <v>175</v>
       </c>
       <c r="C29" t="s">
-        <v>506</v>
+        <v>281</v>
       </c>
       <c r="D29" t="s">
-        <v>420</v>
+        <v>177</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>502</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>504</v>
+        <v>277</v>
       </c>
       <c r="B30" t="s">
-        <v>505</v>
+        <v>175</v>
       </c>
       <c r="C30" t="s">
-        <v>507</v>
+        <v>278</v>
       </c>
       <c r="D30" t="s">
-        <v>420</v>
+        <v>177</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>508</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="B31" t="s">
-        <v>183</v>
+        <v>248</v>
       </c>
       <c r="C31" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="D31" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="B32" t="s">
-        <v>183</v>
+        <v>248</v>
       </c>
       <c r="C32" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="D32" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="B33" t="s">
-        <v>183</v>
+        <v>248</v>
       </c>
       <c r="C33" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="D33" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="B34" t="s">
-        <v>183</v>
+        <v>248</v>
       </c>
       <c r="C34" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="D34" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>271</v>
+        <v>116</v>
       </c>
       <c r="B35" t="s">
-        <v>256</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>276</v>
+        <v>117</v>
       </c>
       <c r="D35" t="s">
-        <v>184</v>
+        <v>118</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="G35" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>273</v>
+        <v>306</v>
       </c>
       <c r="B36" t="s">
-        <v>256</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>277</v>
-      </c>
-      <c r="D36" t="s">
-        <v>184</v>
+        <v>309</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>275</v>
+        <v>307</v>
       </c>
       <c r="B37" t="s">
-        <v>256</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>278</v>
-      </c>
-      <c r="D37" t="s">
-        <v>184</v>
+        <v>310</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>280</v>
+        <v>308</v>
       </c>
       <c r="B38" t="s">
-        <v>256</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>281</v>
-      </c>
-      <c r="D38" t="s">
-        <v>184</v>
+        <v>311</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>116</v>
+        <v>384</v>
       </c>
       <c r="B39" t="s">
         <v>103</v>
       </c>
       <c r="C39" t="s">
-        <v>117</v>
-      </c>
-      <c r="D39" t="s">
+        <v>402</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>385</v>
+      </c>
+      <c r="B40" t="s">
+        <v>175</v>
+      </c>
+      <c r="C40" t="s">
+        <v>403</v>
+      </c>
+      <c r="D40" t="s">
+        <v>99</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>386</v>
+      </c>
+      <c r="B41" t="s">
+        <v>175</v>
+      </c>
+      <c r="C41" t="s">
+        <v>406</v>
+      </c>
+      <c r="D41" t="s">
+        <v>407</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>387</v>
+      </c>
+      <c r="B42" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" t="s">
+        <v>411</v>
+      </c>
+      <c r="D42" t="s">
+        <v>412</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>388</v>
+      </c>
+      <c r="B43" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" t="s">
+        <v>413</v>
+      </c>
+      <c r="D43" t="s">
+        <v>412</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>389</v>
+      </c>
+      <c r="B44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" t="s">
+        <v>415</v>
+      </c>
+      <c r="D44" t="s">
         <v>118</v>
       </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>314</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>390</v>
+      </c>
+      <c r="B45" t="s">
         <v>103</v>
       </c>
-      <c r="C40" t="s">
-        <v>317</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>315</v>
-      </c>
-      <c r="B41" t="s">
-        <v>103</v>
-      </c>
-      <c r="C41" t="s">
-        <v>318</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>316</v>
-      </c>
-      <c r="B42" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" t="s">
-        <v>319</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="F42" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="C45" t="s">
+        <v>416</v>
+      </c>
+      <c r="D45" t="s">
+        <v>118</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>391</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
+        <v>417</v>
+      </c>
+      <c r="D46" t="s">
+        <v>412</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>392</v>
       </c>
-      <c r="B43" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" t="s">
-        <v>410</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" t="s">
+        <v>418</v>
+      </c>
+      <c r="D47" t="s">
+        <v>424</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>425</v>
+      </c>
+      <c r="I47" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>393</v>
       </c>
-      <c r="B44" t="s">
-        <v>183</v>
-      </c>
-      <c r="C44" t="s">
-        <v>411</v>
-      </c>
-      <c r="D44" t="s">
-        <v>99</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-      <c r="F44" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="B48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" t="s">
+        <v>419</v>
+      </c>
+      <c r="D48" t="s">
+        <v>424</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>426</v>
+      </c>
+      <c r="I48" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>394</v>
       </c>
-      <c r="B45" t="s">
-        <v>183</v>
-      </c>
-      <c r="C45" t="s">
-        <v>414</v>
-      </c>
-      <c r="D45" t="s">
-        <v>415</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-      <c r="F45" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="B49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" t="s">
+        <v>420</v>
+      </c>
+      <c r="D49" t="s">
+        <v>424</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>427</v>
+      </c>
+      <c r="I49" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>395</v>
-      </c>
-      <c r="B46" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" t="s">
-        <v>419</v>
-      </c>
-      <c r="D46" t="s">
-        <v>420</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>396</v>
-      </c>
-      <c r="B47" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" t="s">
-        <v>421</v>
-      </c>
-      <c r="D47" t="s">
-        <v>420</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>397</v>
-      </c>
-      <c r="B48" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" t="s">
-        <v>423</v>
-      </c>
-      <c r="D48" t="s">
-        <v>118</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-      <c r="F48" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>398</v>
-      </c>
-      <c r="B49" t="s">
-        <v>103</v>
-      </c>
-      <c r="C49" t="s">
-        <v>424</v>
-      </c>
-      <c r="D49" t="s">
-        <v>118</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-      <c r="F49" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>399</v>
       </c>
       <c r="B50" t="s">
         <v>89</v>
       </c>
       <c r="C50" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="D50" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="E50">
         <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>396</v>
+      </c>
+      <c r="B51" t="s">
+        <v>175</v>
+      </c>
+      <c r="C51" t="s">
+        <v>431</v>
+      </c>
+      <c r="D51" t="s">
+        <v>407</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>397</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" t="s">
+        <v>432</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>398</v>
+      </c>
+      <c r="B53" t="s">
+        <v>175</v>
+      </c>
+      <c r="C53" t="s">
+        <v>433</v>
+      </c>
+      <c r="D53" t="s">
+        <v>407</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>399</v>
+      </c>
+      <c r="B54" t="s">
+        <v>175</v>
+      </c>
+      <c r="C54" t="s">
+        <v>437</v>
+      </c>
+      <c r="D54" t="s">
+        <v>407</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>400</v>
       </c>
-      <c r="B51" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" t="s">
-        <v>426</v>
-      </c>
-      <c r="D51" t="s">
-        <v>432</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="B55" t="s">
+        <v>175</v>
+      </c>
+      <c r="C55" t="s">
+        <v>434</v>
+      </c>
+      <c r="D55" t="s">
+        <v>407</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>401</v>
-      </c>
-      <c r="B52" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" t="s">
-        <v>427</v>
-      </c>
-      <c r="D52" t="s">
-        <v>432</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-      <c r="F52" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>402</v>
-      </c>
-      <c r="B53" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" t="s">
-        <v>428</v>
-      </c>
-      <c r="D53" t="s">
-        <v>432</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-      <c r="F53" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>403</v>
-      </c>
-      <c r="B54" t="s">
-        <v>89</v>
-      </c>
-      <c r="C54" t="s">
-        <v>438</v>
-      </c>
-      <c r="D54" t="s">
-        <v>420</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-      <c r="F54" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>404</v>
-      </c>
-      <c r="B55" t="s">
-        <v>183</v>
-      </c>
-      <c r="C55" t="s">
-        <v>439</v>
-      </c>
-      <c r="D55" t="s">
-        <v>415</v>
-      </c>
-      <c r="E55">
-        <v>1</v>
-      </c>
-      <c r="F55" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>405</v>
       </c>
       <c r="B56" t="s">
         <v>103</v>
       </c>
       <c r="C56" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>406</v>
-      </c>
-      <c r="B57" t="s">
-        <v>183</v>
-      </c>
-      <c r="C57" t="s">
-        <v>441</v>
-      </c>
-      <c r="D57" t="s">
-        <v>415</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-      <c r="F57" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>407</v>
-      </c>
-      <c r="B58" t="s">
-        <v>183</v>
-      </c>
-      <c r="C58" t="s">
-        <v>445</v>
-      </c>
-      <c r="D58" t="s">
-        <v>415</v>
-      </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-      <c r="F58" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>408</v>
-      </c>
-      <c r="B59" t="s">
-        <v>183</v>
-      </c>
-      <c r="C59" t="s">
-        <v>442</v>
-      </c>
-      <c r="D59" t="s">
-        <v>415</v>
-      </c>
-      <c r="E59">
-        <v>1</v>
-      </c>
-      <c r="F59" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>409</v>
-      </c>
-      <c r="B60" t="s">
-        <v>103</v>
-      </c>
-      <c r="C60" t="s">
-        <v>443</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-      <c r="F60" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -3560,8 +3513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75AE531-5F28-4AEB-8C78-A2C7D800AE06}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3581,21 +3534,21 @@
         <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3604,18 +3557,18 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3624,18 +3577,18 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E3" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F3" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3644,18 +3597,18 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E4" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="F4" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3664,18 +3617,18 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E5" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="F5" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3684,18 +3637,18 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E6" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="F6" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3704,18 +3657,18 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" t="s">
+        <v>236</v>
+      </c>
+      <c r="F7" t="s">
         <v>240</v>
-      </c>
-      <c r="E7" t="s">
-        <v>244</v>
-      </c>
-      <c r="F7" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3724,18 +3677,18 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
+        <v>233</v>
+      </c>
+      <c r="E8" t="s">
         <v>241</v>
       </c>
-      <c r="E8" t="s">
-        <v>249</v>
-      </c>
       <c r="F8" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3744,18 +3697,18 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="E9" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="F9" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3764,18 +3717,18 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="E10" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="F10" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3784,18 +3737,18 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="E11" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="F11" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3804,18 +3757,18 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="E12" t="s">
+        <v>237</v>
+      </c>
+      <c r="F12" t="s">
         <v>245</v>
-      </c>
-      <c r="F12" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3824,18 +3777,18 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="E13" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="F13" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3844,18 +3797,18 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="E14" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="F14" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3864,18 +3817,18 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="E15" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="F15" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3884,18 +3837,18 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="E16" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="F16" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3904,18 +3857,18 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="E17" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="F17" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3924,18 +3877,18 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="E18" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="F18" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3944,18 +3897,18 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="E19" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="F19" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3964,18 +3917,18 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="E20" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="F20" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3984,18 +3937,18 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="E21" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="F21" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -4004,15 +3957,15 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F22" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -4021,18 +3974,18 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="E23" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F23" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4041,18 +3994,18 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E24" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F24" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -4061,18 +4014,18 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
+        <v>294</v>
+      </c>
+      <c r="E25" t="s">
+        <v>298</v>
+      </c>
+      <c r="F25" t="s">
         <v>302</v>
-      </c>
-      <c r="E25" t="s">
-        <v>306</v>
-      </c>
-      <c r="F25" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4081,18 +4034,18 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="E26" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="F26" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -4101,18 +4054,18 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="E27" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="F27" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4121,18 +4074,18 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="E28" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="F28" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -4141,18 +4094,18 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E29" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="F29" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -4161,38 +4114,38 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="E30" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="F30" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>321</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>331</v>
+      </c>
+      <c r="E31" t="s">
+        <v>330</v>
+      </c>
+      <c r="F31" t="s">
         <v>329</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>339</v>
-      </c>
-      <c r="E31" t="s">
-        <v>338</v>
-      </c>
-      <c r="F31" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -4201,18 +4154,18 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="E32" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="F32" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -4221,18 +4174,18 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E33" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="F33" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -4241,18 +4194,18 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="E34" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="F34" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -4261,18 +4214,18 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
+        <v>502</v>
+      </c>
+      <c r="E35" t="s">
+        <v>509</v>
+      </c>
+      <c r="F35" t="s">
         <v>510</v>
-      </c>
-      <c r="E35" t="s">
-        <v>517</v>
-      </c>
-      <c r="F35" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -4281,18 +4234,18 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
+        <v>503</v>
+      </c>
+      <c r="E36" t="s">
         <v>511</v>
       </c>
-      <c r="E36" t="s">
-        <v>519</v>
-      </c>
       <c r="F36" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -4301,18 +4254,18 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="E37" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="F37" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -4321,32 +4274,32 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>326</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
         <v>334</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>342</v>
-      </c>
       <c r="E39" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="F39" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -4355,12 +4308,12 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -4369,12 +4322,12 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -4383,18 +4336,18 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="E42" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="F42" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -4403,38 +4356,38 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="E43" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="F43" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>350</v>
+      </c>
+      <c r="E44" t="s">
+        <v>354</v>
+      </c>
+      <c r="F44" t="s">
         <v>355</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44" t="s">
-        <v>358</v>
-      </c>
-      <c r="E44" t="s">
-        <v>362</v>
-      </c>
-      <c r="F44" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -4443,18 +4396,18 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="E45" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="F45" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -4463,18 +4416,18 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="E46" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="F46" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -4483,18 +4436,18 @@
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="E47" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="F47" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -4503,18 +4456,18 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="E48" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="F48" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -4523,13 +4476,13 @@
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="E49" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="F49" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -4554,10 +4507,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -4632,7 +4585,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4645,7 +4598,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -4661,10 +4614,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFFF226-FD8D-405F-AC10-4A4E4C6B33CC}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4672,12 +4625,12 @@
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -4687,110 +4640,113 @@
       <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B2" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>374</v>
       </c>
-      <c r="C3" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>378</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -4800,10 +4756,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454C6314-6461-4ABC-918C-BCDD53997451}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4813,7 +4769,7 @@
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -4823,8 +4779,12 @@
       <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
@@ -4832,59 +4792,64 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>530</v>
       </c>
     </row>
   </sheetData>
@@ -4894,51 +4859,55 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA62531-8327-41AB-8ED0-65EF79FFF446}">
-  <dimension ref="S1:U4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="19" max="19" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="19:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="S1" s="1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="19:21" x14ac:dyDescent="0.3">
-      <c r="S2" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="T2" t="s">
+      <c r="B2" t="s">
         <v>51</v>
       </c>
-      <c r="U2" t="s">
+      <c r="C2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="19:21" x14ac:dyDescent="0.3">
-      <c r="T3" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>52</v>
       </c>
-      <c r="U3" t="s">
+      <c r="C3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="19:21" x14ac:dyDescent="0.3">
-      <c r="U4" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4949,10 +4918,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E40053E-0EA0-4FEA-AACD-B68C4E59D396}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4961,7 +4930,7 @@
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -4971,10 +4940,14 @@
       <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
@@ -4983,7 +4956,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>36</v>
       </c>
@@ -4991,7 +4964,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>40</v>
       </c>
@@ -5003,10 +4976,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C29BB8-DF26-4DBF-9F2A-266DD1D35874}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5016,7 +4989,7 @@
     <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -5026,8 +4999,12 @@
       <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>44</v>
       </c>
@@ -5038,7 +5015,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
@@ -5046,7 +5023,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>56</v>
       </c>
@@ -5054,7 +5031,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>76</v>
       </c>
@@ -5062,7 +5039,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>78</v>
       </c>
@@ -5070,7 +5047,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>77</v>
       </c>
@@ -5078,7 +5055,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>79</v>
       </c>
@@ -5086,7 +5063,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>80</v>
       </c>
@@ -5094,72 +5071,72 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C14" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C15" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -5170,10 +5147,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33BC08A-9C37-4190-BFC8-7F8F9A74425A}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5183,7 +5160,7 @@
     <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -5193,8 +5170,12 @@
       <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -5205,7 +5186,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>72</v>
       </c>
@@ -5217,10 +5198,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C02AF99-CC81-4E23-AD37-6DA0EA50F8B4}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5230,7 +5211,7 @@
     <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -5240,81 +5221,75 @@
       <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C6" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C7" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. log values as strings 2. optimized logging rx as content
</commit_message>
<xml_diff>
--- a/dist/artifacts/msg_enum.xlsx
+++ b/dist/artifacts/msg_enum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWAK_APD_CARE\apdcare\therapy_src\scripts\code_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7CF3D0-5384-4B5B-BDA4-E99D95651CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7E67C0-C7C1-4D7A-8F99-60E705046B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="11" xr2:uid="{9845A9FD-3F8D-4BE4-B40E-983F7B836130}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="532">
   <si>
     <t>thread_cmd</t>
   </si>
@@ -701,12 +701,6 @@
     <t>CCPD_POST_FAN</t>
   </si>
   <si>
-    <t>air</t>
-  </si>
-  <si>
-    <t>fluid</t>
-  </si>
-  <si>
     <t>CCPD_POST_END_MS</t>
   </si>
   <si>
@@ -1667,10 +1661,13 @@
     <t>HT_MODE</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>off</t>
+    <t>system state</t>
+  </si>
+  <si>
+    <t>CCPD_RUNNING_STATE</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_RUNNING_STATE</t>
   </si>
 </sst>
 </file>
@@ -2099,7 +2096,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -2144,7 +2141,7 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
@@ -2163,12 +2160,12 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -2204,10 +2201,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB8DE98-D929-4CE5-A1B4-9DDCBFC59D47}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2229,7 +2226,7 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
@@ -2241,10 +2238,10 @@
         <v>194</v>
       </c>
       <c r="C2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -2255,7 +2252,7 @@
         <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -2263,10 +2260,10 @@
         <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -2274,10 +2271,10 @@
         <v>197</v>
       </c>
       <c r="C5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -2285,10 +2282,10 @@
         <v>198</v>
       </c>
       <c r="C6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -2296,10 +2293,10 @@
         <v>199</v>
       </c>
       <c r="C7" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -2307,10 +2304,10 @@
         <v>200</v>
       </c>
       <c r="C8" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D8" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -2318,7 +2315,7 @@
         <v>201</v>
       </c>
       <c r="C9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -2326,7 +2323,7 @@
         <v>202</v>
       </c>
       <c r="C10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -2334,7 +2331,7 @@
         <v>203</v>
       </c>
       <c r="C11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -2342,7 +2339,7 @@
         <v>204</v>
       </c>
       <c r="C12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -2350,7 +2347,7 @@
         <v>205</v>
       </c>
       <c r="C13" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -2370,7 +2367,12 @@
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>211</v>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>530</v>
       </c>
     </row>
   </sheetData>
@@ -2381,10 +2383,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67343738-2015-487A-BA26-ADA61FE35773}">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2395,7 +2397,7 @@
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
@@ -2414,17 +2416,8 @@
       <c r="F1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G1" s="1">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1">
-        <v>65535</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -2441,7 +2434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -2461,7 +2454,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -2478,7 +2471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>96</v>
       </c>
@@ -2495,7 +2488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -2515,7 +2508,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>102</v>
       </c>
@@ -2532,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -2552,7 +2545,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -2572,7 +2565,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -2592,7 +2585,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>112</v>
       </c>
@@ -2612,7 +2605,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -2632,7 +2625,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -2649,10 +2642,10 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -2669,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -2686,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -2703,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>125</v>
       </c>
@@ -2720,7 +2713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>127</v>
       </c>
@@ -2737,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>151</v>
       </c>
@@ -2757,7 +2750,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>152</v>
       </c>
@@ -2777,7 +2770,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>153</v>
       </c>
@@ -2796,14 +2789,8 @@
       <c r="F21" t="s">
         <v>186</v>
       </c>
-      <c r="G21" t="s">
-        <v>209</v>
-      </c>
-      <c r="H21" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>145</v>
       </c>
@@ -2823,7 +2810,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>146</v>
       </c>
@@ -2843,7 +2830,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>147</v>
       </c>
@@ -2863,55 +2850,55 @@
         <v>187</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>493</v>
+      </c>
+      <c r="B25" t="s">
         <v>495</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>496</v>
+      </c>
+      <c r="D25" t="s">
+        <v>410</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>494</v>
+      </c>
+      <c r="B26" t="s">
+        <v>495</v>
+      </c>
+      <c r="C26" t="s">
         <v>497</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D26" t="s">
+        <v>410</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
         <v>498</v>
       </c>
-      <c r="D25" t="s">
-        <v>412</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>496</v>
-      </c>
-      <c r="B26" t="s">
-        <v>497</v>
-      </c>
-      <c r="C26" t="s">
-        <v>499</v>
-      </c>
-      <c r="D26" t="s">
-        <v>412</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B27" t="s">
         <v>175</v>
       </c>
       <c r="C27" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D27" t="s">
         <v>177</v>
@@ -2920,18 +2907,18 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B28" t="s">
         <v>175</v>
       </c>
       <c r="C28" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D28" t="s">
         <v>177</v>
@@ -2940,18 +2927,18 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B29" t="s">
         <v>175</v>
       </c>
       <c r="C29" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D29" t="s">
         <v>177</v>
@@ -2960,18 +2947,18 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B30" t="s">
         <v>175</v>
       </c>
       <c r="C30" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D30" t="s">
         <v>177</v>
@@ -2980,18 +2967,18 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B31" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D31" t="s">
         <v>176</v>
@@ -3000,18 +2987,18 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B32" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C32" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D32" t="s">
         <v>176</v>
@@ -3020,18 +3007,18 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B33" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C33" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D33" t="s">
         <v>176</v>
@@ -3040,18 +3027,18 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>270</v>
+      </c>
+      <c r="B34" t="s">
+        <v>246</v>
+      </c>
+      <c r="C34" t="s">
         <v>271</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>272</v>
-      </c>
-      <c r="B34" t="s">
-        <v>248</v>
-      </c>
-      <c r="C34" t="s">
-        <v>273</v>
       </c>
       <c r="D34" t="s">
         <v>176</v>
@@ -3060,10 +3047,10 @@
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>116</v>
       </c>
@@ -3080,89 +3067,86 @@
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>291</v>
-      </c>
-      <c r="G35" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B36" t="s">
         <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B37" t="s">
         <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B38" t="s">
         <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B39" t="s">
         <v>103</v>
       </c>
       <c r="C39" t="s">
+        <v>400</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
         <v>402</v>
       </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B40" t="s">
         <v>175</v>
       </c>
       <c r="C40" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D40" t="s">
         <v>99</v>
@@ -3171,78 +3155,78 @@
         <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B41" t="s">
         <v>175</v>
       </c>
       <c r="C41" t="s">
+        <v>404</v>
+      </c>
+      <c r="D41" t="s">
+        <v>405</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
         <v>406</v>
       </c>
-      <c r="D41" t="s">
-        <v>407</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B42" t="s">
         <v>97</v>
       </c>
       <c r="C42" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D42" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B43" t="s">
         <v>97</v>
       </c>
       <c r="C43" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D43" t="s">
+        <v>410</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
         <v>412</v>
       </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B44" t="s">
         <v>103</v>
       </c>
       <c r="C44" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D44" t="s">
         <v>118</v>
@@ -3251,18 +3235,18 @@
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B45" t="s">
         <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D45" t="s">
         <v>118</v>
@@ -3271,230 +3255,238 @@
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B46" t="s">
         <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D46" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B47" t="s">
         <v>89</v>
       </c>
       <c r="C47" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D47" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>425</v>
-      </c>
-      <c r="I47" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B48" t="s">
         <v>89</v>
       </c>
       <c r="C48" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D48" t="s">
+        <v>422</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
         <v>424</v>
       </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-      <c r="F48" t="s">
-        <v>426</v>
-      </c>
-      <c r="I48" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B49" t="s">
         <v>89</v>
       </c>
       <c r="C49" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D49" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E49">
         <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>427</v>
-      </c>
-      <c r="I49" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B50" t="s">
         <v>89</v>
       </c>
       <c r="C50" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D50" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E50">
         <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B51" t="s">
         <v>175</v>
       </c>
       <c r="C51" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D51" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E51">
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B52" t="s">
         <v>103</v>
       </c>
       <c r="C52" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B53" t="s">
         <v>175</v>
       </c>
       <c r="C53" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D53" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E53">
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B54" t="s">
         <v>175</v>
       </c>
       <c r="C54" t="s">
+        <v>435</v>
+      </c>
+      <c r="D54" t="s">
+        <v>405</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
         <v>437</v>
       </c>
-      <c r="D54" t="s">
-        <v>407</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-      <c r="F54" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B55" t="s">
         <v>175</v>
       </c>
       <c r="C55" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D55" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E55">
         <v>1</v>
       </c>
       <c r="F55" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B56" t="s">
         <v>103</v>
       </c>
       <c r="C56" t="s">
-        <v>435</v>
+        <v>433</v>
+      </c>
+      <c r="D56" t="s">
+        <v>118</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>423</v>
+        <v>421</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>531</v>
+      </c>
+      <c r="B57" t="s">
+        <v>495</v>
+      </c>
+      <c r="C57" t="s">
+        <v>529</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3513,8 +3505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75AE531-5F28-4AEB-8C78-A2C7D800AE06}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3588,7 +3580,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3600,15 +3592,15 @@
         <v>162</v>
       </c>
       <c r="E4" t="s">
+        <v>315</v>
+      </c>
+      <c r="F4" t="s">
         <v>317</v>
-      </c>
-      <c r="F4" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3620,15 +3612,15 @@
         <v>162</v>
       </c>
       <c r="E5" t="s">
+        <v>316</v>
+      </c>
+      <c r="F5" t="s">
         <v>318</v>
-      </c>
-      <c r="F5" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3637,18 +3629,18 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3657,18 +3649,18 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3677,18 +3669,18 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3697,18 +3689,18 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" t="s">
+        <v>250</v>
+      </c>
+      <c r="F9" t="s">
         <v>251</v>
-      </c>
-      <c r="E9" t="s">
-        <v>252</v>
-      </c>
-      <c r="F9" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3717,18 +3709,18 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
+        <v>478</v>
+      </c>
+      <c r="E10" t="s">
         <v>480</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>482</v>
-      </c>
-      <c r="F10" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3737,18 +3729,18 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
+        <v>479</v>
+      </c>
+      <c r="E11" t="s">
         <v>481</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>483</v>
-      </c>
-      <c r="F11" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3757,18 +3749,18 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3777,13 +3769,13 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -3797,7 +3789,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E14" t="s">
         <v>180</v>
@@ -3817,7 +3809,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E15" t="s">
         <v>181</v>
@@ -3828,47 +3820,47 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>458</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
         <v>460</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>462</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>464</v>
-      </c>
-      <c r="F16" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>459</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
         <v>461</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>463</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>465</v>
-      </c>
-      <c r="F17" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3877,18 +3869,18 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
+        <v>469</v>
+      </c>
+      <c r="E18" t="s">
         <v>471</v>
       </c>
-      <c r="E18" t="s">
-        <v>473</v>
-      </c>
       <c r="F18" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3897,53 +3889,53 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
+        <v>470</v>
+      </c>
+      <c r="E19" t="s">
+        <v>473</v>
+      </c>
+      <c r="F19" t="s">
         <v>472</v>
-      </c>
-      <c r="E19" t="s">
-        <v>475</v>
-      </c>
-      <c r="F19" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>518</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
         <v>520</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>522</v>
       </c>
-      <c r="E20" t="s">
-        <v>524</v>
-      </c>
       <c r="F20" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>519</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
         <v>521</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>523</v>
-      </c>
       <c r="E21" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F21" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -3965,22 +3957,22 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>446</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>447</v>
+      </c>
+      <c r="E23" t="s">
         <v>448</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="F23" t="s">
         <v>449</v>
-      </c>
-      <c r="E23" t="s">
-        <v>450</v>
-      </c>
-      <c r="F23" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -4005,27 +3997,27 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>290</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
         <v>292</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>294</v>
-      </c>
       <c r="E25" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4034,18 +4026,18 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E26" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F26" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -4054,58 +4046,58 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
+        <v>285</v>
+      </c>
+      <c r="E27" t="s">
+        <v>286</v>
+      </c>
+      <c r="F27" t="s">
         <v>287</v>
-      </c>
-      <c r="E27" t="s">
-        <v>288</v>
-      </c>
-      <c r="F27" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>439</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>440</v>
+      </c>
+      <c r="E28" t="s">
         <v>441</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
         <v>442</v>
-      </c>
-      <c r="E28" t="s">
-        <v>443</v>
-      </c>
-      <c r="F28" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>293</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
         <v>295</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>297</v>
-      </c>
       <c r="E29" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F29" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -4114,18 +4106,18 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E30" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F30" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -4134,18 +4126,18 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E31" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F31" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -4154,18 +4146,18 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E32" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F32" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -4174,18 +4166,18 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E33" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="F33" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -4194,18 +4186,18 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E34" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F34" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -4214,18 +4206,18 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E35" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F35" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -4234,18 +4226,18 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E36" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F36" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -4254,18 +4246,18 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E37" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F37" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -4274,12 +4266,12 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -4288,18 +4280,18 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E39" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F39" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -4308,12 +4300,12 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -4322,12 +4314,12 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -4336,18 +4328,18 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E42" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F42" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -4356,18 +4348,18 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E43" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F43" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -4376,113 +4368,113 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E44" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F44" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>443</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>348</v>
+      </c>
+      <c r="E45" t="s">
+        <v>444</v>
+      </c>
+      <c r="F45" t="s">
         <v>445</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45" t="s">
-        <v>350</v>
-      </c>
-      <c r="E45" t="s">
-        <v>446</v>
-      </c>
-      <c r="F45" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>360</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>361</v>
+      </c>
+      <c r="E46" t="s">
         <v>362</v>
       </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="F46" t="s">
         <v>363</v>
-      </c>
-      <c r="E46" t="s">
-        <v>364</v>
-      </c>
-      <c r="F46" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>450</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
         <v>452</v>
       </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
-        <v>454</v>
-      </c>
       <c r="E47" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F47" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>451</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
         <v>453</v>
       </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-      <c r="D48" t="s">
-        <v>455</v>
-      </c>
       <c r="E48" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F48" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>454</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>455</v>
+      </c>
+      <c r="E49" t="s">
         <v>456</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="F49" t="s">
         <v>457</v>
-      </c>
-      <c r="E49" t="s">
-        <v>458</v>
-      </c>
-      <c r="F49" t="s">
-        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -4585,7 +4577,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4598,7 +4590,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -4641,112 +4633,112 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -4780,7 +4772,7 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
@@ -4849,7 +4841,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
   </sheetData>
@@ -4883,7 +4875,7 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
@@ -4941,13 +4933,13 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
@@ -5000,7 +4992,7 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
@@ -5092,7 +5084,7 @@
         <v>142</v>
       </c>
       <c r="C12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -5100,7 +5092,7 @@
         <v>143</v>
       </c>
       <c r="C13" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -5108,7 +5100,7 @@
         <v>144</v>
       </c>
       <c r="C14" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -5116,7 +5108,7 @@
         <v>191</v>
       </c>
       <c r="C15" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -5131,12 +5123,12 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -5171,7 +5163,7 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
@@ -5222,74 +5214,74 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C6" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C7" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Added new (valve) msgs
</commit_message>
<xml_diff>
--- a/dist/artifacts/msg_enum.xlsx
+++ b/dist/artifacts/msg_enum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWAK_APD_CARE\apdcare\therapy_src\scripts\code_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081287AC-237A-4CC2-8C95-773AE39BC0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F8197E-B6CC-49A5-9508-D6D6ED94202F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="11" xr2:uid="{9845A9FD-3F8D-4BE4-B40E-983F7B836130}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="12" xr2:uid="{9845A9FD-3F8D-4BE4-B40E-983F7B836130}"/>
   </bookViews>
   <sheets>
     <sheet name="threads" sheetId="2" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="560">
   <si>
     <t>thread_cmd</t>
   </si>
@@ -1728,6 +1728,30 @@
   </si>
   <si>
     <t>disp_heater_min_pwm_dc</t>
+  </si>
+  <si>
+    <t>MSG_VALVE_SET_MOVE_DURATION</t>
+  </si>
+  <si>
+    <t>trig_valve_set_dur</t>
+  </si>
+  <si>
+    <t>valve duration updated</t>
+  </si>
+  <si>
+    <t>valve duration set fail</t>
+  </si>
+  <si>
+    <t>trig_set_valve_cont</t>
+  </si>
+  <si>
+    <t>valve seq movement set</t>
+  </si>
+  <si>
+    <t>valve seq movement fail</t>
+  </si>
+  <si>
+    <t>MSG_VALVE_SET_CONT_MOVEMENT</t>
   </si>
 </sst>
 </file>
@@ -2445,8 +2469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67343738-2015-487A-BA26-ADA61FE35773}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3583,10 +3607,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75AE531-5F28-4AEB-8C78-A2C7D800AE06}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4559,7 +4583,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>358</v>
+        <v>559</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -4568,18 +4592,18 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>359</v>
+        <v>556</v>
       </c>
       <c r="E50" t="s">
-        <v>360</v>
+        <v>557</v>
       </c>
       <c r="F50" t="s">
-        <v>361</v>
+        <v>558</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>448</v>
+        <v>552</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -4588,18 +4612,18 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>450</v>
+        <v>553</v>
       </c>
       <c r="E51" t="s">
-        <v>360</v>
+        <v>554</v>
       </c>
       <c r="F51" t="s">
-        <v>361</v>
+        <v>555</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>449</v>
+        <v>358</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -4608,7 +4632,7 @@
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>451</v>
+        <v>359</v>
       </c>
       <c r="E52" t="s">
         <v>360</v>
@@ -4619,21 +4643,61 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>448</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>450</v>
+      </c>
+      <c r="E53" t="s">
+        <v>360</v>
+      </c>
+      <c r="F53" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>449</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>451</v>
+      </c>
+      <c r="E54" t="s">
+        <v>360</v>
+      </c>
+      <c r="F54" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>452</v>
       </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
         <v>453</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E55" t="s">
         <v>454</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F55" t="s">
         <v>455</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1. Added msg priority 2. flexible dash cards
</commit_message>
<xml_diff>
--- a/dist/artifacts/msg_enum.xlsx
+++ b/dist/artifacts/msg_enum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWAK_APD_CARE\apdcare\therapy_src\scripts\code_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F8197E-B6CC-49A5-9508-D6D6ED94202F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FDF150-6A20-4513-9A7E-5B790CC5610A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="12" xr2:uid="{9845A9FD-3F8D-4BE4-B40E-983F7B836130}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="10" xr2:uid="{9845A9FD-3F8D-4BE4-B40E-983F7B836130}"/>
   </bookViews>
   <sheets>
     <sheet name="threads" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <sheet name="event_log_type" sheetId="11" r:id="rId13"/>
     <sheet name="mod_status" sheetId="12" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="554">
   <si>
     <t>thread_cmd</t>
   </si>
@@ -1133,18 +1133,6 @@
     <t>status</t>
   </si>
   <si>
-    <t>CCPD_POST</t>
-  </si>
-  <si>
-    <t>CCPD_SYSCHK</t>
-  </si>
-  <si>
-    <t>CCPD_CALIB</t>
-  </si>
-  <si>
-    <t>CCPD_PRIME</t>
-  </si>
-  <si>
     <t>STATUS</t>
   </si>
   <si>
@@ -1466,15 +1454,6 @@
     <t>Turb side gain failed</t>
   </si>
   <si>
-    <t>CCPD_FILL</t>
-  </si>
-  <si>
-    <t>CCPD_DWELL</t>
-  </si>
-  <si>
-    <t>CCPD_DRAIN</t>
-  </si>
-  <si>
     <t>trig_set_turb_top_inttime</t>
   </si>
   <si>
@@ -1752,6 +1731,9 @@
   </si>
   <si>
     <t>MSG_VALVE_SET_CONT_MOVEMENT</t>
+  </si>
+  <si>
+    <t>CCPD</t>
   </si>
 </sst>
 </file>
@@ -2244,12 +2226,12 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -2287,8 +2269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB8DE98-D929-4CE5-A1B4-9DDCBFC59D47}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2325,7 +2307,7 @@
         <v>209</v>
       </c>
       <c r="D2" t="s">
-        <v>353</v>
+        <v>553</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -2335,9 +2317,6 @@
       <c r="C3" t="s">
         <v>65</v>
       </c>
-      <c r="D3" t="s">
-        <v>354</v>
-      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -2346,9 +2325,6 @@
       <c r="C4" t="s">
         <v>213</v>
       </c>
-      <c r="D4" t="s">
-        <v>355</v>
-      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -2357,19 +2333,13 @@
       <c r="C5" t="s">
         <v>216</v>
       </c>
-      <c r="D5" t="s">
-        <v>356</v>
-      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>196</v>
       </c>
       <c r="C6" t="s">
-        <v>509</v>
-      </c>
-      <c r="D6" t="s">
-        <v>464</v>
+        <v>502</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -2377,10 +2347,7 @@
         <v>197</v>
       </c>
       <c r="C7" t="s">
-        <v>510</v>
-      </c>
-      <c r="D7" t="s">
-        <v>465</v>
+        <v>503</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -2388,10 +2355,7 @@
         <v>198</v>
       </c>
       <c r="C8" t="s">
-        <v>511</v>
-      </c>
-      <c r="D8" t="s">
-        <v>466</v>
+        <v>504</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -2456,7 +2420,7 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -2555,7 +2519,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2714,19 +2678,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="B13" t="s">
         <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -2956,42 +2920,42 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="B26" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="C26" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="D26" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="B27" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="C27" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="D27" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -3227,30 +3191,30 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B40" t="s">
         <v>101</v>
       </c>
       <c r="C40" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B41" t="s">
         <v>173</v>
       </c>
       <c r="C41" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D41" t="s">
         <v>97</v>
@@ -3259,78 +3223,78 @@
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B42" t="s">
         <v>173</v>
       </c>
       <c r="C42" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D42" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B43" t="s">
         <v>95</v>
       </c>
       <c r="C43" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D43" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B44" t="s">
         <v>95</v>
       </c>
       <c r="C44" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D44" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B45" t="s">
         <v>101</v>
       </c>
       <c r="C45" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D45" t="s">
         <v>116</v>
@@ -3339,18 +3303,18 @@
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B46" t="s">
         <v>101</v>
       </c>
       <c r="C46" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D46" t="s">
         <v>116</v>
@@ -3359,215 +3323,215 @@
         <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B47" t="s">
         <v>87</v>
       </c>
       <c r="C47" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D47" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B48" t="s">
         <v>87</v>
       </c>
       <c r="C48" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D48" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E48">
         <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B49" t="s">
         <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D49" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E49">
         <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B50" t="s">
         <v>87</v>
       </c>
       <c r="C50" t="s">
+        <v>412</v>
+      </c>
+      <c r="D50" t="s">
         <v>416</v>
       </c>
-      <c r="D50" t="s">
-        <v>420</v>
-      </c>
       <c r="E50">
         <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B51" t="s">
         <v>87</v>
       </c>
       <c r="C51" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="D51" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E51">
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B52" t="s">
         <v>173</v>
       </c>
       <c r="C52" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D52" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B53" t="s">
         <v>101</v>
       </c>
       <c r="C53" t="s">
+        <v>424</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
         <v>428</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-      <c r="F53" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B54" t="s">
         <v>173</v>
       </c>
       <c r="C54" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D54" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="E54">
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B55" t="s">
         <v>173</v>
       </c>
       <c r="C55" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D55" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="E55">
         <v>1</v>
       </c>
       <c r="F55" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B56" t="s">
         <v>173</v>
       </c>
       <c r="C56" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="D56" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B57" t="s">
         <v>101</v>
       </c>
       <c r="C57" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="D57" t="s">
         <v>116</v>
@@ -3576,18 +3540,18 @@
         <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="B58" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="C58" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -3609,7 +3573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75AE531-5F28-4AEB-8C78-A2C7D800AE06}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -3804,7 +3768,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3813,18 +3777,18 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="E10" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="F10" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3833,13 +3797,13 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="E11" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="F11" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -3924,47 +3888,47 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>452</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>454</v>
+      </c>
+      <c r="E16" t="s">
         <v>456</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>458</v>
-      </c>
-      <c r="E16" t="s">
-        <v>460</v>
-      </c>
-      <c r="F16" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>453</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>455</v>
+      </c>
+      <c r="E17" t="s">
         <v>457</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="F17" t="s">
         <v>459</v>
-      </c>
-      <c r="E17" t="s">
-        <v>461</v>
-      </c>
-      <c r="F17" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3973,18 +3937,18 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="E18" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F18" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3993,18 +3957,18 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E19" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="F19" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -4013,18 +3977,18 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="E20" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="F20" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -4033,13 +3997,13 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="E21" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="F21" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -4061,7 +4025,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -4070,18 +4034,18 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="E23" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="F23" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4090,13 +4054,13 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="E24" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="F24" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -4121,7 +4085,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4130,18 +4094,18 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="E26" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="F26" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -4150,13 +4114,13 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="E27" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="F27" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -4170,7 +4134,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="E28" t="s">
         <v>294</v>
@@ -4221,7 +4185,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -4230,18 +4194,18 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="E31" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="F31" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -4250,13 +4214,13 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E32" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="F32" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -4333,7 +4297,7 @@
         <v>328</v>
       </c>
       <c r="E36" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="F36" t="s">
         <v>331</v>
@@ -4353,15 +4317,15 @@
         <v>336</v>
       </c>
       <c r="E37" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="F37" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -4370,18 +4334,18 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
+        <v>490</v>
+      </c>
+      <c r="E38" t="s">
+        <v>496</v>
+      </c>
+      <c r="F38" t="s">
         <v>497</v>
-      </c>
-      <c r="E38" t="s">
-        <v>503</v>
-      </c>
-      <c r="F38" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -4390,18 +4354,18 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
+        <v>491</v>
+      </c>
+      <c r="E39" t="s">
         <v>498</v>
       </c>
-      <c r="E39" t="s">
-        <v>505</v>
-      </c>
       <c r="F39" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -4410,13 +4374,13 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="E40" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="F40" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -4563,7 +4527,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -4575,15 +4539,15 @@
         <v>346</v>
       </c>
       <c r="E49" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="F49" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -4592,18 +4556,18 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="E50" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="F50" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -4612,18 +4576,18 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="E51" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="F51" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -4632,18 +4596,18 @@
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E52" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F52" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -4652,18 +4616,18 @@
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="E53" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F53" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -4672,18 +4636,18 @@
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="E54" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F54" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -4692,13 +4656,13 @@
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="E55" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="F55" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -4740,7 +4704,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4801,7 +4765,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4814,7 +4778,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -4874,7 +4838,7 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C3" t="s">
         <v>280</v>
@@ -4882,87 +4846,87 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -5065,7 +5029,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
     </row>
   </sheetData>
@@ -5116,7 +5080,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -5305,7 +5269,7 @@
         <v>140</v>
       </c>
       <c r="C12" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -5313,7 +5277,7 @@
         <v>141</v>
       </c>
       <c r="C13" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -5321,7 +5285,7 @@
         <v>142</v>
       </c>
       <c r="C14" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -5329,7 +5293,7 @@
         <v>189</v>
       </c>
       <c r="C15" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -5344,12 +5308,12 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -5479,7 +5443,7 @@
         <v>258</v>
       </c>
       <c r="C6" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -5487,7 +5451,7 @@
         <v>251</v>
       </c>
       <c r="C7" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
1. Updated py datatypes in excel
</commit_message>
<xml_diff>
--- a/dist/artifacts/msg_enum.xlsx
+++ b/dist/artifacts/msg_enum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWAK_APD_CARE\apdcare\therapy_src\scripts\code_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FDF150-6A20-4513-9A7E-5B790CC5610A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CC9EE7-8972-44B6-9C9D-84D9097088CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="10" xr2:uid="{9845A9FD-3F8D-4BE4-B40E-983F7B836130}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="11" xr2:uid="{9845A9FD-3F8D-4BE4-B40E-983F7B836130}"/>
   </bookViews>
   <sheets>
     <sheet name="threads" sheetId="2" r:id="rId1"/>
@@ -32,6 +32,13 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -72,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="572">
   <si>
     <t>thread_cmd</t>
   </si>
@@ -320,9 +327,6 @@
     <t>msg_id</t>
   </si>
   <si>
-    <t>ctype</t>
-  </si>
-  <si>
     <t>datalog_column_name</t>
   </si>
   <si>
@@ -335,9 +339,6 @@
     <t>MSG_HEATER_GET_RUN_INTERVAL</t>
   </si>
   <si>
-    <t>uint16</t>
-  </si>
-  <si>
     <t>heater run interval</t>
   </si>
   <si>
@@ -359,9 +360,6 @@
     <t>MSG_HEATER_GET_TARGET_FLUID_TEMP</t>
   </si>
   <si>
-    <t>int16</t>
-  </si>
-  <si>
     <t>target fluid temp</t>
   </si>
   <si>
@@ -377,9 +375,6 @@
     <t>MSG_HEATER_GET_ADC_LPF_WIN_SIZE</t>
   </si>
   <si>
-    <t>uint8</t>
-  </si>
-  <si>
     <t>heater adc lpf size</t>
   </si>
   <si>
@@ -455,9 +450,6 @@
     <t>bubble sample time</t>
   </si>
   <si>
-    <t>expect_timestamp</t>
-  </si>
-  <si>
     <t>dom_trigger_id</t>
   </si>
   <si>
@@ -593,9 +585,6 @@
     <t>DISABLE_PERITONITIS</t>
   </si>
   <si>
-    <t>float32</t>
-  </si>
-  <si>
     <t>raw</t>
   </si>
   <si>
@@ -806,9 +795,6 @@
     <t>load cell 2 pressure</t>
   </si>
   <si>
-    <t>int32</t>
-  </si>
-  <si>
     <t>disp_lc1_pa</t>
   </si>
   <si>
@@ -1532,9 +1518,6 @@
     <t>MSG_SENSORS_GET_CURRENT_H2_VAL</t>
   </si>
   <si>
-    <t>uint32</t>
-  </si>
-  <si>
     <t>hpad1 current</t>
   </si>
   <si>
@@ -1734,6 +1717,84 @@
   </si>
   <si>
     <t>CCPD</t>
+  </si>
+  <si>
+    <t>MSG_HEATER_ASSERT_ERROR</t>
+  </si>
+  <si>
+    <t>MSG_MAINPUMP_ASSERT_ERROR</t>
+  </si>
+  <si>
+    <t>MSG_VALVE_ASSERT_ERROR</t>
+  </si>
+  <si>
+    <t>MSG_SENSORS_ASSERT_ERROR</t>
+  </si>
+  <si>
+    <t>MSG_BMS_ASSERT_ERROR</t>
+  </si>
+  <si>
+    <t>MSG_LOGGER_ASSERT_ERROR</t>
+  </si>
+  <si>
+    <t>MSG_PRESSURE_ASSERT_ERROR</t>
+  </si>
+  <si>
+    <t>MSG_UI_COMM_ASSERT_ERROR</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_ASSERT_ERROR</t>
+  </si>
+  <si>
+    <t>Heater assert error</t>
+  </si>
+  <si>
+    <t>Mainpump assert error</t>
+  </si>
+  <si>
+    <t>Valve assert error</t>
+  </si>
+  <si>
+    <t>Sensors assert error</t>
+  </si>
+  <si>
+    <t>Logger assert error</t>
+  </si>
+  <si>
+    <t>Pressure assert error</t>
+  </si>
+  <si>
+    <t>BMS assert error</t>
+  </si>
+  <si>
+    <t>Comm assert error</t>
+  </si>
+  <si>
+    <t>UC Master assert error</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>BBH</t>
+  </si>
+  <si>
+    <t>datatype</t>
   </si>
 </sst>
 </file>
@@ -2162,7 +2223,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -2207,7 +2268,7 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
@@ -2226,12 +2287,12 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -2269,7 +2330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB8DE98-D929-4CE5-A1B4-9DDCBFC59D47}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2292,7 +2353,7 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
@@ -2301,18 +2362,18 @@
         <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D2" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
         <v>65</v>
@@ -2320,107 +2381,107 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C5" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C6" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C7" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C8" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C9" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C10" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C11" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C12" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C13" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -2431,10 +2492,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67343738-2015-487A-BA26-ADA61FE35773}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2450,33 +2511,33 @@
         <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>564</v>
+      </c>
+      <c r="C2" t="s">
         <v>86</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>87</v>
-      </c>
-      <c r="C2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" t="s">
-        <v>89</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2484,56 +2545,56 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>566</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" t="s">
         <v>94</v>
-      </c>
-      <c r="B5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" t="s">
-        <v>97</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2541,36 +2602,36 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>566</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2578,153 +2639,153 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>566</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>566</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>566</v>
       </c>
       <c r="C10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>566</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s">
+        <v>565</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" t="s">
         <v>112</v>
       </c>
-      <c r="B12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" t="s">
-        <v>116</v>
-      </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C13" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
+        <v>564</v>
+      </c>
+      <c r="C15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" t="s">
         <v>87</v>
-      </c>
-      <c r="C15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D15" t="s">
-        <v>89</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2732,16 +2793,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B16" t="s">
+        <v>564</v>
+      </c>
+      <c r="C16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" t="s">
         <v>87</v>
-      </c>
-      <c r="C16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16" t="s">
-        <v>89</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -2749,16 +2810,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B17" t="s">
+        <v>564</v>
+      </c>
+      <c r="C17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" t="s">
         <v>87</v>
-      </c>
-      <c r="C17" t="s">
-        <v>122</v>
-      </c>
-      <c r="D17" t="s">
-        <v>89</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2766,16 +2827,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2783,16 +2844,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s">
+        <v>564</v>
+      </c>
+      <c r="C19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" t="s">
         <v>87</v>
-      </c>
-      <c r="C19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" t="s">
-        <v>89</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -2800,770 +2861,864 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>564</v>
       </c>
       <c r="C20" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D20" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" t="s">
+        <v>564</v>
+      </c>
+      <c r="C21" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" t="s">
         <v>150</v>
       </c>
-      <c r="B21" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" t="s">
-        <v>153</v>
-      </c>
-      <c r="D21" t="s">
-        <v>155</v>
-      </c>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B22" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D22" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C23" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D23" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C24" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C25" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D25" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="B26" t="s">
-        <v>486</v>
+        <v>567</v>
       </c>
       <c r="C26" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="D26" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="B27" t="s">
-        <v>486</v>
+        <v>567</v>
       </c>
       <c r="C27" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="D27" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="B28" t="s">
-        <v>173</v>
+        <v>568</v>
       </c>
       <c r="C28" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D28" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="B29" t="s">
-        <v>173</v>
+        <v>568</v>
       </c>
       <c r="C29" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D29" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="B30" t="s">
-        <v>173</v>
+        <v>568</v>
       </c>
       <c r="C30" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="D30" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B31" t="s">
-        <v>173</v>
+        <v>568</v>
       </c>
       <c r="C31" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="D31" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="B32" t="s">
-        <v>244</v>
+        <v>569</v>
       </c>
       <c r="C32" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D32" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B33" t="s">
-        <v>244</v>
+        <v>569</v>
       </c>
       <c r="C33" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="D33" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B34" t="s">
-        <v>244</v>
+        <v>569</v>
       </c>
       <c r="C34" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D34" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="B35" t="s">
-        <v>244</v>
+        <v>569</v>
       </c>
       <c r="C35" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D35" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C36" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D36" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C37" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C38" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C39" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C40" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="B41" t="s">
-        <v>173</v>
+        <v>568</v>
       </c>
       <c r="C41" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="D41" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>568</v>
       </c>
       <c r="C42" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="D42" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>566</v>
       </c>
       <c r="C43" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="D43" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="B44" t="s">
-        <v>95</v>
+        <v>566</v>
       </c>
       <c r="C44" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="D44" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C45" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="D45" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C46" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="D46" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>564</v>
       </c>
       <c r="C47" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="D47" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B48" t="s">
-        <v>87</v>
+        <v>564</v>
       </c>
       <c r="C48" t="s">
+        <v>403</v>
+      </c>
+      <c r="D48" t="s">
+        <v>409</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
         <v>410</v>
-      </c>
-      <c r="D48" t="s">
-        <v>416</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-      <c r="F48" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="B49" t="s">
-        <v>87</v>
+        <v>564</v>
       </c>
       <c r="C49" t="s">
+        <v>404</v>
+      </c>
+      <c r="D49" t="s">
+        <v>409</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
         <v>411</v>
-      </c>
-      <c r="D49" t="s">
-        <v>416</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-      <c r="F49" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B50" t="s">
-        <v>87</v>
+        <v>564</v>
       </c>
       <c r="C50" t="s">
+        <v>405</v>
+      </c>
+      <c r="D50" t="s">
+        <v>409</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
         <v>412</v>
-      </c>
-      <c r="D50" t="s">
-        <v>416</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B51" t="s">
-        <v>87</v>
+        <v>564</v>
       </c>
       <c r="C51" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="D51" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="E51">
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B52" t="s">
-        <v>173</v>
+        <v>568</v>
       </c>
       <c r="C52" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="D52" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="B53" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C53" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="E53">
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="B54" t="s">
-        <v>173</v>
+        <v>568</v>
       </c>
       <c r="C54" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="D54" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="E54">
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="B55" t="s">
-        <v>173</v>
+        <v>568</v>
       </c>
       <c r="C55" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="D55" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="E55">
         <v>1</v>
       </c>
       <c r="F55" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>385</v>
+      </c>
+      <c r="B56" t="s">
+        <v>568</v>
+      </c>
+      <c r="C56" t="s">
+        <v>419</v>
+      </c>
+      <c r="D56" t="s">
         <v>392</v>
       </c>
-      <c r="B56" t="s">
-        <v>173</v>
-      </c>
-      <c r="C56" t="s">
-        <v>426</v>
-      </c>
-      <c r="D56" t="s">
-        <v>399</v>
-      </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B57" t="s">
-        <v>101</v>
+        <v>565</v>
       </c>
       <c r="C57" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="D57" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E57">
         <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="B58" t="s">
-        <v>486</v>
+        <v>567</v>
       </c>
       <c r="C58" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>546</v>
+      </c>
+      <c r="B59" t="s">
+        <v>570</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>547</v>
+      </c>
+      <c r="B60" t="s">
+        <v>570</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>548</v>
+      </c>
+      <c r="B61" t="s">
+        <v>570</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>549</v>
+      </c>
+      <c r="B62" t="s">
+        <v>570</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>550</v>
+      </c>
+      <c r="B63" t="s">
+        <v>570</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>551</v>
+      </c>
+      <c r="B64" t="s">
+        <v>570</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>552</v>
+      </c>
+      <c r="B65" t="s">
+        <v>570</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>553</v>
+      </c>
+      <c r="B66" t="s">
+        <v>570</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>554</v>
+      </c>
+      <c r="B67" t="s">
+        <v>570</v>
+      </c>
+      <c r="E67">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{48FF53FC-FB56-47DC-A3E5-5D20D2AD4BFF}">
-      <formula1>"int8, uint8, int16, uint16, int32, uint32, float32, bool, void"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -3571,1098 +3726,1063 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75AE531-5F28-4AEB-8C78-A2C7D800AE06}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E3" t="s">
         <v>131</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>1</v>
+      <c r="C4" t="s">
+        <v>155</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>306</v>
       </c>
       <c r="E4" t="s">
-        <v>313</v>
-      </c>
-      <c r="F4" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>1</v>
+      <c r="C5" t="s">
+        <v>155</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>307</v>
       </c>
       <c r="E5" t="s">
-        <v>314</v>
-      </c>
-      <c r="F5" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>222</v>
+      </c>
+      <c r="D7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" t="s">
+        <v>231</v>
+      </c>
+      <c r="E8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D9" t="s">
+        <v>241</v>
+      </c>
+      <c r="E9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>468</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>462</v>
+      </c>
+      <c r="D10" t="s">
+        <v>464</v>
+      </c>
+      <c r="E10" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>469</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>463</v>
+      </c>
+      <c r="D11" t="s">
+        <v>465</v>
+      </c>
+      <c r="E11" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
         <v>224</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="D12" t="s">
+        <v>227</v>
+      </c>
+      <c r="E12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>224</v>
+      </c>
+      <c r="D13" t="s">
         <v>228</v>
-      </c>
-      <c r="E6" t="s">
-        <v>231</v>
-      </c>
-      <c r="F6" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>228</v>
-      </c>
-      <c r="E7" t="s">
-        <v>232</v>
-      </c>
-      <c r="F7" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>239</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>229</v>
-      </c>
-      <c r="E8" t="s">
-        <v>237</v>
-      </c>
-      <c r="F8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>250</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>247</v>
-      </c>
-      <c r="E9" t="s">
-        <v>248</v>
-      </c>
-      <c r="F9" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>475</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>469</v>
-      </c>
-      <c r="E10" t="s">
-        <v>471</v>
-      </c>
-      <c r="F10" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>476</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>470</v>
-      </c>
-      <c r="E11" t="s">
-        <v>472</v>
-      </c>
-      <c r="F11" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>226</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>230</v>
-      </c>
-      <c r="E12" t="s">
-        <v>233</v>
-      </c>
-      <c r="F12" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>227</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>230</v>
       </c>
       <c r="E13" t="s">
         <v>234</v>
       </c>
-      <c r="F13" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14">
-        <v>1</v>
+      <c r="C14" t="s">
+        <v>202</v>
       </c>
       <c r="D14" t="s">
-        <v>208</v>
+        <v>172</v>
       </c>
       <c r="E14" t="s">
-        <v>178</v>
-      </c>
-      <c r="F14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15">
-        <v>1</v>
+      <c r="C15" t="s">
+        <v>202</v>
       </c>
       <c r="D15" t="s">
-        <v>208</v>
+        <v>173</v>
       </c>
       <c r="E15" t="s">
-        <v>179</v>
-      </c>
-      <c r="F15" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>445</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>447</v>
+      </c>
+      <c r="D16" t="s">
+        <v>449</v>
+      </c>
+      <c r="E16" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>446</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>448</v>
+      </c>
+      <c r="D17" t="s">
+        <v>450</v>
+      </c>
+      <c r="E17" t="s">
         <v>452</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>458</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>453</v>
+      </c>
+      <c r="D18" t="s">
+        <v>455</v>
+      </c>
+      <c r="E18" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>459</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>454</v>
       </c>
-      <c r="E16" t="s">
+      <c r="D19" t="s">
+        <v>457</v>
+      </c>
+      <c r="E19" t="s">
         <v>456</v>
       </c>
-      <c r="F16" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>453</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>455</v>
-      </c>
-      <c r="E17" t="s">
-        <v>457</v>
-      </c>
-      <c r="F17" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>465</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>460</v>
-      </c>
-      <c r="E18" t="s">
-        <v>462</v>
-      </c>
-      <c r="F18" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>466</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>461</v>
-      </c>
-      <c r="E19" t="s">
-        <v>464</v>
-      </c>
-      <c r="F19" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20">
-        <v>1</v>
+      <c r="C20" t="s">
+        <v>503</v>
       </c>
       <c r="D20" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="E20" t="s">
-        <v>513</v>
-      </c>
-      <c r="F20" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21">
-        <v>1</v>
+      <c r="C21" t="s">
+        <v>504</v>
       </c>
       <c r="D21" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="E21" t="s">
-        <v>515</v>
-      </c>
-      <c r="F21" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22">
-        <v>1</v>
+      <c r="D22" t="s">
+        <v>133</v>
       </c>
       <c r="E22" t="s">
-        <v>138</v>
-      </c>
-      <c r="F22" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23">
-        <v>1</v>
+      <c r="C23" t="s">
+        <v>434</v>
       </c>
       <c r="D23" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="E23" t="s">
-        <v>442</v>
-      </c>
-      <c r="F23" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>527</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>526</v>
+      </c>
+      <c r="D24" t="s">
+        <v>524</v>
+      </c>
+      <c r="E24" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" t="s">
+        <v>165</v>
+      </c>
+      <c r="E25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>528</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>529</v>
+      </c>
+      <c r="D26" t="s">
+        <v>530</v>
+      </c>
+      <c r="E26" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>535</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>532</v>
+      </c>
+      <c r="D27" t="s">
+        <v>533</v>
+      </c>
+      <c r="E27" t="s">
         <v>534</v>
       </c>
-      <c r="E24" t="s">
-        <v>532</v>
-      </c>
-      <c r="F24" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>168</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>167</v>
-      </c>
-      <c r="E25" t="s">
-        <v>170</v>
-      </c>
-      <c r="F25" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>536</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>537</v>
-      </c>
-      <c r="E26" t="s">
-        <v>538</v>
-      </c>
-      <c r="F26" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>543</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>540</v>
-      </c>
-      <c r="E27" t="s">
-        <v>541</v>
-      </c>
-      <c r="F27" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28">
-        <v>1</v>
+      <c r="C28" t="s">
+        <v>523</v>
       </c>
       <c r="D28" t="s">
-        <v>531</v>
+        <v>287</v>
       </c>
       <c r="E28" t="s">
-        <v>294</v>
-      </c>
-      <c r="F28" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
-      <c r="C29">
-        <v>1</v>
+      <c r="C29" t="s">
+        <v>283</v>
       </c>
       <c r="D29" t="s">
+        <v>288</v>
+      </c>
+      <c r="E29" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>279</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>276</v>
+      </c>
+      <c r="D30" t="s">
+        <v>277</v>
+      </c>
+      <c r="E30" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>519</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>516</v>
+      </c>
+      <c r="D31" t="s">
+        <v>517</v>
+      </c>
+      <c r="E31" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>426</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>427</v>
+      </c>
+      <c r="D32" t="s">
+        <v>428</v>
+      </c>
+      <c r="E32" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>284</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>286</v>
+      </c>
+      <c r="D33" t="s">
+        <v>289</v>
+      </c>
+      <c r="E33" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>285</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>333</v>
+      </c>
+      <c r="D34" t="s">
         <v>290</v>
       </c>
-      <c r="E29" t="s">
-        <v>295</v>
-      </c>
-      <c r="F29" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>286</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>283</v>
-      </c>
-      <c r="E30" t="s">
-        <v>284</v>
-      </c>
-      <c r="F30" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>527</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>524</v>
-      </c>
-      <c r="E31" t="s">
-        <v>525</v>
-      </c>
-      <c r="F31" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>433</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>434</v>
-      </c>
-      <c r="E32" t="s">
-        <v>435</v>
-      </c>
-      <c r="F32" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>291</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>293</v>
-      </c>
-      <c r="E33" t="s">
-        <v>296</v>
-      </c>
-      <c r="F33" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>292</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>340</v>
-      </c>
       <c r="E34" t="s">
-        <v>297</v>
-      </c>
-      <c r="F34" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35">
-        <v>1</v>
+      <c r="C35" t="s">
+        <v>320</v>
       </c>
       <c r="D35" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="E35" t="s">
-        <v>326</v>
-      </c>
-      <c r="F35" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36">
-        <v>1</v>
+      <c r="C36" t="s">
+        <v>321</v>
       </c>
       <c r="D36" t="s">
-        <v>328</v>
+        <v>487</v>
       </c>
       <c r="E36" t="s">
-        <v>495</v>
-      </c>
-      <c r="F36" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37">
-        <v>1</v>
+      <c r="C37" t="s">
+        <v>329</v>
       </c>
       <c r="D37" t="s">
-        <v>336</v>
+        <v>485</v>
       </c>
       <c r="E37" t="s">
-        <v>493</v>
-      </c>
-      <c r="F37" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
-      <c r="C38">
-        <v>1</v>
+      <c r="C38" t="s">
+        <v>482</v>
       </c>
       <c r="D38" t="s">
+        <v>488</v>
+      </c>
+      <c r="E38" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>498</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>483</v>
+      </c>
+      <c r="D39" t="s">
         <v>490</v>
       </c>
-      <c r="E38" t="s">
-        <v>496</v>
-      </c>
-      <c r="F38" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>506</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>491</v>
       </c>
-      <c r="E39" t="s">
-        <v>498</v>
-      </c>
-      <c r="F39" t="s">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>507</v>
-      </c>
       <c r="B40">
         <v>1</v>
       </c>
-      <c r="C40">
-        <v>1</v>
+      <c r="C40" t="s">
+        <v>484</v>
       </c>
       <c r="D40" t="s">
         <v>492</v>
       </c>
       <c r="E40" t="s">
-        <v>500</v>
-      </c>
-      <c r="F40" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
-      <c r="C41">
-        <v>1</v>
+      <c r="C41" t="s">
+        <v>322</v>
       </c>
       <c r="D41" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E41" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>314</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>315</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>323</v>
+      </c>
+      <c r="D43" t="s">
+        <v>327</v>
+      </c>
+      <c r="E43" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>316</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>317</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
         <v>332</v>
       </c>
-      <c r="F41" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>321</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>334</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>322</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>330</v>
-      </c>
-      <c r="E43" t="s">
-        <v>334</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="D46" t="s">
+        <v>340</v>
+      </c>
+      <c r="E46" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>323</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>324</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
+        <v>342</v>
+      </c>
+      <c r="E47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>336</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>341</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="D48" t="s">
+        <v>343</v>
+      </c>
+      <c r="E48" t="s">
         <v>344</v>
       </c>
-      <c r="E46" t="s">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>430</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>339</v>
+      </c>
+      <c r="D49" t="s">
+        <v>431</v>
+      </c>
+      <c r="E49" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>544</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>541</v>
+      </c>
+      <c r="D50" t="s">
+        <v>542</v>
+      </c>
+      <c r="E50" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>537</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>538</v>
+      </c>
+      <c r="D51" t="s">
+        <v>539</v>
+      </c>
+      <c r="E51" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>347</v>
       </c>
-      <c r="F46" t="s">
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>342</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
-        <v>345</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="D52" t="s">
         <v>349</v>
       </c>
-      <c r="F47" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>343</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-      <c r="D48" t="s">
-        <v>346</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="E52" t="s">
         <v>350</v>
       </c>
-      <c r="F48" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>437</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49" t="s">
-        <v>346</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>439</v>
+      </c>
+      <c r="D53" t="s">
+        <v>349</v>
+      </c>
+      <c r="E53" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>438</v>
       </c>
-      <c r="F49" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>440</v>
+      </c>
+      <c r="D54" t="s">
+        <v>349</v>
+      </c>
+      <c r="E54" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>441</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>442</v>
+      </c>
+      <c r="D55" t="s">
+        <v>443</v>
+      </c>
+      <c r="E55" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>546</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>555</v>
+      </c>
+      <c r="E56" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>547</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>556</v>
+      </c>
+      <c r="E57" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>548</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>557</v>
+      </c>
+      <c r="E58" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>549</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>558</v>
+      </c>
+      <c r="E59" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>550</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
+        <v>561</v>
+      </c>
+      <c r="E60" t="str">
+        <f>D60</f>
+        <v>BMS assert error</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>551</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>559</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" ref="E61:E64" si="0">D61</f>
+        <v>Logger assert error</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>552</v>
       </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="D50" t="s">
-        <v>549</v>
-      </c>
-      <c r="E50" t="s">
-        <v>550</v>
-      </c>
-      <c r="F50" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>545</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51" t="s">
-        <v>546</v>
-      </c>
-      <c r="E51" t="s">
-        <v>547</v>
-      </c>
-      <c r="F51" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>354</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52" t="s">
-        <v>355</v>
-      </c>
-      <c r="E52" t="s">
-        <v>356</v>
-      </c>
-      <c r="F52" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>444</v>
-      </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53" t="s">
-        <v>446</v>
-      </c>
-      <c r="E53" t="s">
-        <v>356</v>
-      </c>
-      <c r="F53" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>445</v>
-      </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54" t="s">
-        <v>447</v>
-      </c>
-      <c r="E54" t="s">
-        <v>356</v>
-      </c>
-      <c r="F54" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>448</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55" t="s">
-        <v>449</v>
-      </c>
-      <c r="E55" t="s">
-        <v>450</v>
-      </c>
-      <c r="F55" t="s">
-        <v>451</v>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>560</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="0"/>
+        <v>Pressure assert error</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>553</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>562</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="0"/>
+        <v>Comm assert error</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>554</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>563</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="0"/>
+        <v>UC Master assert error</v>
       </c>
     </row>
   </sheetData>
@@ -4687,10 +4807,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -4765,7 +4885,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4778,7 +4898,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -4821,112 +4941,112 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="C3" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -4960,7 +5080,7 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
@@ -5029,7 +5149,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
     </row>
   </sheetData>
@@ -5063,7 +5183,7 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
@@ -5080,7 +5200,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -5118,13 +5238,13 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
@@ -5177,7 +5297,7 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
@@ -5253,7 +5373,7 @@
         <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -5261,59 +5381,59 @@
         <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C14" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C15" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -5348,7 +5468,7 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
@@ -5399,74 +5519,74 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C4" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C6" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C7" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>